<commit_message>
made the colors for the test
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/eclipse-workspace/Clue/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978D53CE-0F93-1745-8C61-1BB649A8D4C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25048F5E-977B-7E4D-8832-4AB0B2AAB467}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="500" windowWidth="27980" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9420" yWindow="500" windowWidth="19380" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClueLayout" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,6 +232,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -245,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -257,6 +269,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,7 +733,7 @@
       <c r="U2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="15" t="s">
         <v>34</v>
       </c>
       <c r="X2" s="10" t="s">
@@ -745,7 +762,7 @@
       <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -760,7 +777,7 @@
       <c r="L3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N3" s="3" t="s">
@@ -802,7 +819,7 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -974,7 +991,7 @@
       <c r="M6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="O6" s="1" t="s">
@@ -1009,7 +1026,7 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1024,7 +1041,7 @@
       <c r="F7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -1095,7 +1112,7 @@
       <c r="F8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="3" t="s">
@@ -1122,7 +1139,7 @@
       <c r="O8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="11" t="s">
         <v>13</v>
       </c>
       <c r="Q8" s="3" t="s">
@@ -1137,7 +1154,7 @@
       <c r="T8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="U8" s="3" t="s">
+      <c r="U8" s="14" t="s">
         <v>3</v>
       </c>
       <c r="V8" s="3" t="s">
@@ -1148,7 +1165,7 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1208,7 +1225,7 @@
       <c r="U9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="V9" s="3" t="s">
+      <c r="V9" s="12" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1234,7 +1251,7 @@
       <c r="G10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="11" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1249,7 +1266,7 @@
       <c r="L10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N10" s="3" t="s">
@@ -1302,7 +1319,7 @@
       <c r="G11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="12" t="s">
         <v>3</v>
       </c>
       <c r="I11" s="3" t="s">
@@ -1406,13 +1423,13 @@
       <c r="S12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T12" s="3" t="s">
+      <c r="T12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="V12" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1462,7 +1479,7 @@
       <c r="O13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q13" s="1" t="s">
@@ -1524,7 +1541,7 @@
       <c r="M14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="N14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="O14" s="1" t="s">
@@ -1545,7 +1562,7 @@
       <c r="T14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="U14" s="5" t="s">
+      <c r="U14" s="15" t="s">
         <v>32</v>
       </c>
       <c r="V14" s="1" t="s">
@@ -1728,7 +1745,7 @@
       <c r="M17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="N17" s="13" t="s">
         <v>3</v>
       </c>
       <c r="O17" s="1" t="s">
@@ -1950,7 +1967,7 @@
       <c r="S20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T20" s="3" t="s">
+      <c r="T20" s="11" t="s">
         <v>12</v>
       </c>
       <c r="U20" s="1" t="s">
@@ -2012,7 +2029,7 @@
       <c r="Q21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R21" s="3" t="s">
+      <c r="R21" s="11" t="s">
         <v>14</v>
       </c>
       <c r="S21" s="3" t="s">
@@ -2109,7 +2126,7 @@
       <c r="D23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -2121,7 +2138,7 @@
       <c r="H23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J23" s="3" t="s">
@@ -2136,7 +2153,7 @@
       <c r="M23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="N23" s="6" t="s">
         <v>17</v>
       </c>
       <c r="O23" s="1" t="s">
@@ -2260,7 +2277,7 @@
       <c r="I25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="J25" s="14" t="s">
         <v>12</v>
       </c>
       <c r="K25" s="1" t="s">
@@ -2304,7 +2321,7 @@
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="1" t="s">

</xml_diff>

<commit_message>
Changed data files to reflect room label layout aesthetics
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/eclipse-workspace/Clue/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/eclipse-workspace/clue/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25048F5E-977B-7E4D-8832-4AB0B2AAB467}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A862526-8404-E24D-BD33-3FFFC7F9B613}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="500" windowWidth="19380" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="19380" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClueLayout" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="43">
   <si>
     <t>B</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Red: test occupied</t>
+  </si>
+  <si>
+    <t>H#</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
   <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -838,7 +841,7 @@
         <v>2</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>2</v>
@@ -1359,10 +1362,10 @@
         <v>3</v>
       </c>
       <c r="U11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V11" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -1373,7 +1376,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
@@ -1409,13 +1412,13 @@
         <v>3</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>8</v>
@@ -1444,7 +1447,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>7</v>
@@ -1835,10 +1838,10 @@
         <v>9</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
@@ -1903,7 +1906,7 @@
         <v>9</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="V19" s="1" t="s">
         <v>9</v>
@@ -2121,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>6</v>
@@ -2148,7 +2151,7 @@
         <v>5</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>5</v>
@@ -2160,7 +2163,7 @@
         <v>5</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>5</v>
@@ -2192,7 +2195,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>6</v>

</xml_diff>